<commit_message>
For now, compustat data are always always not significant. More work need to be done
</commit_message>
<xml_diff>
--- a/Data/Quarterly.xlsx
+++ b/Data/Quarterly.xlsx
@@ -1508,10 +1508,10 @@
   <dimension ref="A1:CL937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="CD210" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="CD198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="CL221" sqref="CL221:CL279"/>
+      <selection pane="bottomRight" activeCell="CK226" sqref="CK226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -47573,12 +47573,6 @@
       <c r="CJ221" s="3">
         <v>2.06129259198671E-2</v>
       </c>
-      <c r="CK221" s="3">
-        <v>-1.3604810000000001</v>
-      </c>
-      <c r="CL221" s="3">
-        <v>-1.092444</v>
-      </c>
     </row>
     <row r="222" spans="2:90">
       <c r="B222" s="4">
@@ -47843,12 +47837,6 @@
       <c r="CJ222" s="3">
         <v>3.18737972655697E-2</v>
       </c>
-      <c r="CK222" s="3">
-        <v>-91.748068000000004</v>
-      </c>
-      <c r="CL222" s="3">
-        <v>-109.832984</v>
-      </c>
     </row>
     <row r="223" spans="2:90">
       <c r="B223" s="4">
@@ -48112,12 +48100,6 @@
       </c>
       <c r="CJ223" s="3">
         <v>3.52516450914791E-2</v>
-      </c>
-      <c r="CK223" s="3">
-        <v>-243.46148400000001</v>
-      </c>
-      <c r="CL223" s="3">
-        <v>-284.05667</v>
       </c>
     </row>
     <row r="224" spans="2:90">

</xml_diff>